<commit_message>
G41-63 #comment Completing the self assessment
</commit_message>
<xml_diff>
--- a/LAPR3-2021-Self-Assessment.xlsx
+++ b/LAPR3-2021-Self-Assessment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Desktop\Universidade-ISEP\2ANO\LAPR3\ProjetoIntegrador_G41\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96494EAE-430F-4172-8523-35D4B1F3B97F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5AB71A5-089B-47B4-B035-D99D7E881EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{5ECC33D7-267E-3941-AADB-18CFA00ADDCE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5ECC33D7-267E-3941-AADB-18CFA00ADDCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="2" r:id="rId1"/>
@@ -2076,8 +2076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A51149F-37F8-9041-812D-F0949B9CB00F}">
   <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2256,12 +2256,24 @@
       <c r="C11" s="8">
         <v>1201276</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
+      <c r="D11" s="9">
+        <v>5</v>
+      </c>
+      <c r="E11" s="39">
+        <v>5</v>
+      </c>
+      <c r="F11" s="38">
+        <v>5</v>
+      </c>
+      <c r="G11" s="8">
+        <v>5</v>
+      </c>
+      <c r="H11" s="8">
+        <v>3</v>
+      </c>
+      <c r="I11" s="8">
+        <v>5</v>
+      </c>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
@@ -2271,9 +2283,9 @@
       <c r="P11" s="8"/>
       <c r="Q11" s="8"/>
       <c r="R11" s="10"/>
-      <c r="S11" s="54" t="e">
+      <c r="S11" s="54">
         <f t="shared" ref="S11:S24" si="0">AVERAGE(D11:R11)</f>
-        <v>#DIV/0!</v>
+        <v>4.666666666666667</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2656,27 +2668,27 @@
       </c>
       <c r="D25" s="49">
         <f>AVERAGE(D10:D24)</f>
-        <v>4.4000000000000004</v>
+        <v>4.5</v>
       </c>
       <c r="E25" s="49">
         <f t="shared" ref="E25:R25" si="1">AVERAGE(E10:E24)</f>
-        <v>4.8</v>
+        <v>4.833333333333333</v>
       </c>
       <c r="F25" s="49">
         <f t="shared" si="1"/>
-        <v>4.8</v>
+        <v>4.833333333333333</v>
       </c>
       <c r="G25" s="49">
         <f t="shared" si="1"/>
-        <v>4.4000000000000004</v>
+        <v>4.5</v>
       </c>
       <c r="H25" s="49">
         <f t="shared" si="1"/>
-        <v>3.4</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="I25" s="49">
         <f t="shared" si="1"/>
-        <v>4.5999999999999996</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="J25" s="49" t="e">
         <f t="shared" si="1"/>
@@ -3724,7 +3736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20984BA6-2128-EB41-A750-F94245E6A6D5}">
   <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
G41-98 #comment Adding self assessment file
</commit_message>
<xml_diff>
--- a/LAPR3-2021-Self-Assessment.xlsx
+++ b/LAPR3-2021-Self-Assessment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Desktop\Universidade-ISEP\2ANO\LAPR3\ProjetoIntegrador_G41\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5AB71A5-089B-47B4-B035-D99D7E881EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92AC110B-1050-4CC1-A7A0-6AF9C88AD0F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5ECC33D7-267E-3941-AADB-18CFA00ADDCE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{5ECC33D7-267E-3941-AADB-18CFA00ADDCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="164">
   <si>
     <t>Fill the cells with a blue background</t>
   </si>
@@ -188,43 +188,10 @@
     <t>The students have exceeded expectations </t>
   </si>
   <si>
-    <t>US101</t>
-  </si>
-  <si>
     <t>The students  have exceeded expectations </t>
   </si>
   <si>
-    <t>US102</t>
-  </si>
-  <si>
-    <t>US103</t>
-  </si>
-  <si>
-    <t>US104</t>
-  </si>
-  <si>
-    <t>US105</t>
-  </si>
-  <si>
-    <t>US106</t>
-  </si>
-  <si>
-    <t>US107</t>
-  </si>
-  <si>
-    <t>US108</t>
-  </si>
-  <si>
-    <t>US109</t>
-  </si>
-  <si>
-    <t>US110</t>
-  </si>
-  <si>
     <t>US111</t>
-  </si>
-  <si>
-    <t>US112</t>
   </si>
   <si>
     <t>Code Quality based on Sonarqube Data</t>
@@ -572,6 +539,42 @@
   </si>
   <si>
     <t>LAPR3 Project Group and Self-assessment v1.0</t>
+  </si>
+  <si>
+    <t>Student 5</t>
+  </si>
+  <si>
+    <t>Student 6</t>
+  </si>
+  <si>
+    <t>US201</t>
+  </si>
+  <si>
+    <t>US202</t>
+  </si>
+  <si>
+    <t>US203</t>
+  </si>
+  <si>
+    <t>US204</t>
+  </si>
+  <si>
+    <t>US205</t>
+  </si>
+  <si>
+    <t>US206</t>
+  </si>
+  <si>
+    <t>US207</t>
+  </si>
+  <si>
+    <t>US208</t>
+  </si>
+  <si>
+    <t>US209</t>
+  </si>
+  <si>
+    <t>US210</t>
   </si>
 </sst>
 </file>
@@ -2076,8 +2079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A51149F-37F8-9041-812D-F0949B9CB00F}">
   <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2090,7 +2093,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2164,13 +2167,13 @@
         <f>C13</f>
         <v>1201384</v>
       </c>
-      <c r="H9" s="46">
+      <c r="H9" s="46" t="str">
         <f>C14</f>
-        <v>1180727</v>
-      </c>
-      <c r="I9" s="46">
+        <v>Student 5</v>
+      </c>
+      <c r="I9" s="46" t="str">
         <f>C15</f>
-        <v>1200801</v>
+        <v>Student 6</v>
       </c>
       <c r="J9" s="46" t="str">
         <f>C16</f>
@@ -2231,12 +2234,8 @@
       <c r="G10" s="42">
         <v>5</v>
       </c>
-      <c r="H10" s="42">
-        <v>4</v>
-      </c>
-      <c r="I10" s="42">
-        <v>4</v>
-      </c>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
       <c r="J10" s="42"/>
       <c r="K10" s="42"/>
       <c r="L10" s="42"/>
@@ -2248,7 +2247,7 @@
       <c r="R10" s="40"/>
       <c r="S10" s="53">
         <f>AVERAGE(D10:R10)</f>
-        <v>4.5</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2268,12 +2267,8 @@
       <c r="G11" s="8">
         <v>5</v>
       </c>
-      <c r="H11" s="8">
-        <v>3</v>
-      </c>
-      <c r="I11" s="8">
-        <v>5</v>
-      </c>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
@@ -2285,7 +2280,7 @@
       <c r="R11" s="10"/>
       <c r="S11" s="54">
         <f t="shared" ref="S11:S24" si="0">AVERAGE(D11:R11)</f>
-        <v>4.666666666666667</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2294,7 +2289,7 @@
         <v>1201381</v>
       </c>
       <c r="D12" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E12" s="9">
         <v>5</v>
@@ -2303,14 +2298,10 @@
         <v>5</v>
       </c>
       <c r="G12" s="38">
-        <v>4</v>
-      </c>
-      <c r="H12" s="8">
-        <v>3</v>
-      </c>
-      <c r="I12" s="8">
-        <v>5</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
@@ -2322,7 +2313,7 @@
       <c r="R12" s="10"/>
       <c r="S12" s="54">
         <f t="shared" si="0"/>
-        <v>4.333333333333333</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2340,14 +2331,10 @@
         <v>5</v>
       </c>
       <c r="G13" s="39">
-        <v>4</v>
-      </c>
-      <c r="H13" s="38">
-        <v>3</v>
-      </c>
-      <c r="I13" s="8">
-        <v>5</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="H13" s="38"/>
+      <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
@@ -2359,32 +2346,20 @@
       <c r="R13" s="10"/>
       <c r="S13" s="54">
         <f t="shared" si="0"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="76"/>
-      <c r="C14" s="8">
-        <v>1180727</v>
-      </c>
-      <c r="D14" s="8">
-        <v>5</v>
-      </c>
-      <c r="E14" s="8">
-        <v>5</v>
-      </c>
-      <c r="F14" s="8">
-        <v>5</v>
-      </c>
-      <c r="G14" s="9">
-        <v>5</v>
-      </c>
-      <c r="H14" s="39">
-        <v>3</v>
-      </c>
-      <c r="I14" s="38">
-        <v>5</v>
-      </c>
+      <c r="C14" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="38"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
@@ -2394,34 +2369,22 @@
       <c r="P14" s="8"/>
       <c r="Q14" s="8"/>
       <c r="R14" s="10"/>
-      <c r="S14" s="54">
+      <c r="S14" s="54" t="e">
         <f t="shared" si="0"/>
-        <v>4.666666666666667</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="76"/>
-      <c r="C15" s="8">
-        <v>1200801</v>
-      </c>
-      <c r="D15" s="8">
-        <v>4</v>
-      </c>
-      <c r="E15" s="8">
-        <v>4</v>
-      </c>
-      <c r="F15" s="8">
-        <v>4</v>
-      </c>
-      <c r="G15" s="8">
-        <v>4</v>
-      </c>
-      <c r="H15" s="9">
-        <v>4</v>
-      </c>
-      <c r="I15" s="39">
-        <v>4</v>
-      </c>
+      <c r="C15" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="39"/>
       <c r="J15" s="38"/>
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
@@ -2431,9 +2394,9 @@
       <c r="P15" s="8"/>
       <c r="Q15" s="8"/>
       <c r="R15" s="10"/>
-      <c r="S15" s="54">
+      <c r="S15" s="54" t="e">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2668,27 +2631,27 @@
       </c>
       <c r="D25" s="49">
         <f>AVERAGE(D10:D24)</f>
-        <v>4.5</v>
+        <v>4.75</v>
       </c>
       <c r="E25" s="49">
         <f t="shared" ref="E25:R25" si="1">AVERAGE(E10:E24)</f>
-        <v>4.833333333333333</v>
+        <v>5</v>
       </c>
       <c r="F25" s="49">
         <f t="shared" si="1"/>
-        <v>4.833333333333333</v>
+        <v>5</v>
       </c>
       <c r="G25" s="49">
         <f t="shared" si="1"/>
-        <v>4.5</v>
-      </c>
-      <c r="H25" s="49">
+        <v>5</v>
+      </c>
+      <c r="H25" s="49" t="e">
         <f t="shared" si="1"/>
-        <v>3.3333333333333335</v>
-      </c>
-      <c r="I25" s="49">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I25" s="49" t="e">
         <f t="shared" si="1"/>
-        <v>4.666666666666667</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="J25" s="49" t="e">
         <f t="shared" si="1"/>
@@ -2815,8 +2778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049E9D47-BAA1-5945-9716-C25FEE03B60C}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2915,7 +2878,7 @@
     </row>
     <row r="6" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>43</v>
+        <v>154</v>
       </c>
       <c r="B6" s="8">
         <v>1201381</v>
@@ -2940,15 +2903,15 @@
         <v>41</v>
       </c>
       <c r="J6" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>45</v>
+        <v>155</v>
       </c>
       <c r="B7" s="8">
-        <v>1201384</v>
+        <v>1201276</v>
       </c>
       <c r="C7" s="8">
         <v>5</v>
@@ -2970,12 +2933,12 @@
         <v>41</v>
       </c>
       <c r="J7" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>46</v>
+        <v>156</v>
       </c>
       <c r="B8" s="8">
         <v>1201276</v>
@@ -3000,15 +2963,15 @@
         <v>41</v>
       </c>
       <c r="J8" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>47</v>
+        <v>157</v>
       </c>
       <c r="B9" s="8">
-        <v>1201381</v>
+        <v>1170504</v>
       </c>
       <c r="C9" s="8">
         <v>5</v>
@@ -3030,15 +2993,15 @@
         <v>41</v>
       </c>
       <c r="J9" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>48</v>
+        <v>158</v>
       </c>
       <c r="B10" s="8">
-        <v>1180727</v>
+        <v>1201276</v>
       </c>
       <c r="C10" s="8">
         <v>5</v>
@@ -3060,15 +3023,15 @@
         <v>41</v>
       </c>
       <c r="J10" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>49</v>
+        <v>159</v>
       </c>
       <c r="B11" s="8">
-        <v>1180727</v>
+        <v>1201384</v>
       </c>
       <c r="C11" s="8">
         <v>5</v>
@@ -3090,15 +3053,15 @@
         <v>41</v>
       </c>
       <c r="J11" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>50</v>
+        <v>160</v>
       </c>
       <c r="B12" s="8">
-        <v>1201276</v>
+        <v>1170504</v>
       </c>
       <c r="C12" s="8">
         <v>5</v>
@@ -3120,15 +3083,15 @@
         <v>41</v>
       </c>
       <c r="J12" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>51</v>
+        <v>161</v>
       </c>
       <c r="B13" s="8">
-        <v>1200801</v>
+        <v>1201381</v>
       </c>
       <c r="C13" s="8">
         <v>5</v>
@@ -3150,15 +3113,15 @@
         <v>41</v>
       </c>
       <c r="J13" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>52</v>
+        <v>162</v>
       </c>
       <c r="B14" s="8">
-        <v>1201384</v>
+        <v>1201276</v>
       </c>
       <c r="C14" s="8">
         <v>5</v>
@@ -3180,15 +3143,15 @@
         <v>41</v>
       </c>
       <c r="J14" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>53</v>
+        <v>163</v>
       </c>
       <c r="B15" s="8">
-        <v>1200801</v>
+        <v>1201384</v>
       </c>
       <c r="C15" s="8">
         <v>5</v>
@@ -3210,16 +3173,18 @@
         <v>41</v>
       </c>
       <c r="J15" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" s="8"/>
+        <v>44</v>
+      </c>
+      <c r="B16" s="8">
+        <v>1201381</v>
+      </c>
       <c r="C16" s="8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D16" s="13"/>
       <c r="E16" s="15" t="s">
@@ -3238,13 +3203,11 @@
         <v>41</v>
       </c>
       <c r="J16" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
-        <v>55</v>
-      </c>
+      <c r="A17" s="15"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="13"/>
@@ -3264,7 +3227,7 @@
         <v>41</v>
       </c>
       <c r="J17" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -3288,7 +3251,7 @@
         <v>41</v>
       </c>
       <c r="J18" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -3312,7 +3275,7 @@
         <v>41</v>
       </c>
       <c r="J19" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -3336,7 +3299,7 @@
         <v>41</v>
       </c>
       <c r="J20" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -3360,7 +3323,7 @@
         <v>41</v>
       </c>
       <c r="J21" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -3384,7 +3347,7 @@
         <v>41</v>
       </c>
       <c r="J22" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -3408,7 +3371,7 @@
         <v>41</v>
       </c>
       <c r="J23" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -3432,7 +3395,7 @@
         <v>41</v>
       </c>
       <c r="J24" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -3456,7 +3419,7 @@
         <v>41</v>
       </c>
       <c r="J25" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -3580,7 +3543,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3591,39 +3554,39 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="33" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="60" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B3" s="59" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C3" s="57" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D3" s="57" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E3" s="57" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F3" s="58" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="61" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B4" s="11">
         <v>34</v>
       </c>
       <c r="C4" s="64">
-        <v>96.1</v>
+        <v>89.9</v>
       </c>
       <c r="D4" s="22">
         <v>80</v>
@@ -3633,39 +3596,39 @@
       </c>
       <c r="F4" s="12">
         <f>IF(((C4-D4)/(E4-D4)*100)&gt;100,100,(C4-D4)/(E4-D4)*100)</f>
-        <v>100</v>
+        <v>99.000000000000057</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B5" s="15">
         <v>21</v>
       </c>
       <c r="C5" s="31">
-        <v>75.400000000000006</v>
+        <v>73.400000000000006</v>
       </c>
       <c r="D5" s="7">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E5" s="7">
         <v>85</v>
       </c>
       <c r="F5" s="16">
         <f>IF(((C5-D5)/(E5-D5)*100)&gt;100,100,(C5-D5)/(E5-D5)*100)</f>
-        <v>4.0000000000000568</v>
+        <v>42.000000000000028</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="62" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B6" s="15">
         <v>-13</v>
       </c>
       <c r="C6" s="30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D6" s="7">
         <v>5</v>
@@ -3680,13 +3643,13 @@
     </row>
     <row r="7" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="63" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B7" s="23">
         <v>-13</v>
       </c>
       <c r="C7" s="65">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" s="24">
         <v>5</v>
@@ -3701,7 +3664,7 @@
     </row>
     <row r="8" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="48" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B8" s="57">
         <v>55</v>
@@ -3711,7 +3674,7 @@
       <c r="E8" s="57"/>
       <c r="F8" s="58">
         <f>SUMPRODUCT(B4:B7,F4:F7)/100</f>
-        <v>34.840000000000011</v>
+        <v>42.480000000000025</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3720,11 +3683,11 @@
       <c r="C9" s="67"/>
       <c r="D9" s="68"/>
       <c r="E9" s="48" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="F9" s="69">
         <f>IF((F8/B8)&lt;0,0,(F8/B8))</f>
-        <v>0.6334545454545456</v>
+        <v>0.77236363636363681</v>
       </c>
     </row>
   </sheetData>
@@ -3737,7 +3700,7 @@
   <dimension ref="A1:Z11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3759,7 +3722,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -3779,10 +3742,10 @@
     <row r="2" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C3" s="21">
         <f>'Group and Self Assessment'!C10</f>
@@ -3800,13 +3763,13 @@
         <f>'Group and Self Assessment'!C13</f>
         <v>1201384</v>
       </c>
-      <c r="G3" s="21">
+      <c r="G3" s="21" t="str">
         <f>'Group and Self Assessment'!C14</f>
-        <v>1180727</v>
-      </c>
-      <c r="H3" s="21">
+        <v>Student 5</v>
+      </c>
+      <c r="H3" s="21" t="str">
         <f>'Group and Self Assessment'!C15</f>
-        <v>1200801</v>
+        <v>Student 6</v>
       </c>
       <c r="I3" s="21" t="str">
         <f>'Group and Self Assessment'!C16</f>
@@ -3872,7 +3835,7 @@
         <v>5</v>
       </c>
       <c r="Y3" s="22" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="Z3" s="12" t="s">
         <v>30</v>
@@ -3880,105 +3843,105 @@
     </row>
     <row r="4" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B4" s="18">
         <v>0.35</v>
       </c>
       <c r="C4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>3.1672727272727279</v>
+        <v>3.861818181818184</v>
       </c>
       <c r="D4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>3.1672727272727279</v>
+        <v>3.861818181818184</v>
       </c>
       <c r="E4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>3.1672727272727279</v>
+        <v>3.861818181818184</v>
       </c>
       <c r="F4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>3.1672727272727279</v>
+        <v>3.861818181818184</v>
       </c>
       <c r="G4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>3.1672727272727279</v>
+        <v>3.861818181818184</v>
       </c>
       <c r="H4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>3.1672727272727279</v>
+        <v>3.861818181818184</v>
       </c>
       <c r="I4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>3.1672727272727279</v>
+        <v>3.861818181818184</v>
       </c>
       <c r="J4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>3.1672727272727279</v>
+        <v>3.861818181818184</v>
       </c>
       <c r="K4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>3.1672727272727279</v>
+        <v>3.861818181818184</v>
       </c>
       <c r="L4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>3.1672727272727279</v>
+        <v>3.861818181818184</v>
       </c>
       <c r="M4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>3.1672727272727279</v>
+        <v>3.861818181818184</v>
       </c>
       <c r="N4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>3.1672727272727279</v>
+        <v>3.861818181818184</v>
       </c>
       <c r="O4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>3.1672727272727279</v>
+        <v>3.861818181818184</v>
       </c>
       <c r="P4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>3.1672727272727279</v>
+        <v>3.861818181818184</v>
       </c>
       <c r="Q4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>3.1672727272727279</v>
+        <v>3.861818181818184</v>
       </c>
       <c r="R4" s="28">
         <f>AVERAGE(C4:Q4)</f>
-        <v>3.1672727272727288</v>
+        <v>3.8618181818181849</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="T4" s="7" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="U4" s="7" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="W4" s="7" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="X4" s="7" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="Y4" s="7"/>
       <c r="Z4" s="16"/>
     </row>
     <row r="5" spans="1:26" ht="63" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B5" s="18">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="C5" s="26">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D5" s="26">
         <v>5</v>
@@ -4006,32 +3969,32 @@
       <c r="Q5" s="26"/>
       <c r="R5" s="28">
         <f t="shared" ref="R5:R8" si="0">AVERAGE(C5:Q5)</f>
-        <v>4.333333333333333</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="T5" s="7" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="V5" s="7" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="W5" s="7" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="X5" s="7" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="Y5" s="7"/>
       <c r="Z5" s="16"/>
     </row>
     <row r="6" spans="1:26" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B6" s="18">
         <v>0.1</v>
@@ -4068,29 +4031,29 @@
         <v>5</v>
       </c>
       <c r="S6" s="7" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="T6" s="7" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="V6" s="7" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="W6" s="7" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="X6" s="7" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="Y6" s="7"/>
       <c r="Z6" s="16"/>
     </row>
     <row r="7" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B7" s="18">
         <v>0.35</v>
@@ -4127,29 +4090,29 @@
         <v>4.166666666666667</v>
       </c>
       <c r="S7" s="7" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="U7" s="7" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="V7" s="7" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="W7" s="7" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="X7" s="7" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="Y7" s="7"/>
       <c r="Z7" s="16"/>
     </row>
     <row r="8" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B8" s="18">
         <v>0.125</v>
@@ -4186,29 +4149,29 @@
         <v>5</v>
       </c>
       <c r="S8" s="7" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="T8" s="7" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="U8" s="7" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="V8" s="7" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="W8" s="7" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="X8" s="7" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="Y8" s="7"/>
       <c r="Z8" s="16"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B9" s="19">
         <f>SUM(B4:B8)</f>
@@ -4216,63 +4179,63 @@
       </c>
       <c r="C9" s="7">
         <f>SUMPRODUCT(C4:C8,$B$4:$B$8)</f>
-        <v>3.8585454545454545</v>
+        <v>4.251636363636365</v>
       </c>
       <c r="D9" s="7">
         <f t="shared" ref="D9:Q9" si="1">SUMPRODUCT(D4:D8,$B$4:$B$8)</f>
-        <v>4.0085454545454544</v>
+        <v>4.251636363636365</v>
       </c>
       <c r="E9" s="7">
         <f t="shared" si="1"/>
-        <v>4.0085454545454544</v>
+        <v>4.251636363636365</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="1"/>
-        <v>3.8585454545454545</v>
+        <v>4.1016363636363646</v>
       </c>
       <c r="G9" s="7">
         <f t="shared" si="1"/>
-        <v>4.0085454545454544</v>
+        <v>4.251636363636365</v>
       </c>
       <c r="H9" s="7">
         <f t="shared" si="1"/>
-        <v>4.3585454545454549</v>
+        <v>4.6016363636363646</v>
       </c>
       <c r="I9" s="7">
         <f t="shared" si="1"/>
-        <v>1.1085454545454547</v>
+        <v>1.3516363636363644</v>
       </c>
       <c r="J9" s="7">
         <f t="shared" si="1"/>
-        <v>1.1085454545454547</v>
+        <v>1.3516363636363644</v>
       </c>
       <c r="K9" s="7">
         <f t="shared" si="1"/>
-        <v>1.1085454545454547</v>
+        <v>1.3516363636363644</v>
       </c>
       <c r="L9" s="7">
         <f t="shared" si="1"/>
-        <v>1.1085454545454547</v>
+        <v>1.3516363636363644</v>
       </c>
       <c r="M9" s="7">
         <f t="shared" si="1"/>
-        <v>1.1085454545454547</v>
+        <v>1.3516363636363644</v>
       </c>
       <c r="N9" s="7">
         <f t="shared" si="1"/>
-        <v>1.1085454545454547</v>
+        <v>1.3516363636363644</v>
       </c>
       <c r="O9" s="7">
         <f t="shared" si="1"/>
-        <v>1.1085454545454547</v>
+        <v>1.3516363636363644</v>
       </c>
       <c r="P9" s="7">
         <f t="shared" si="1"/>
-        <v>1.1085454545454547</v>
+        <v>1.3516363636363644</v>
       </c>
       <c r="Q9" s="7">
         <f t="shared" si="1"/>
-        <v>1.1085454545454547</v>
+        <v>1.3516363636363644</v>
       </c>
       <c r="R9" s="28"/>
       <c r="S9" s="7"/>
@@ -4286,68 +4249,68 @@
     </row>
     <row r="10" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B10" s="24"/>
       <c r="C10" s="24">
         <f>C9/5*20</f>
-        <v>15.434181818181818</v>
+        <v>17.00654545454546</v>
       </c>
       <c r="D10" s="24">
         <f t="shared" ref="D10:Q10" si="2">D9/5*20</f>
-        <v>16.034181818181818</v>
+        <v>17.00654545454546</v>
       </c>
       <c r="E10" s="24">
         <f t="shared" si="2"/>
-        <v>16.034181818181818</v>
+        <v>17.00654545454546</v>
       </c>
       <c r="F10" s="24">
         <f t="shared" si="2"/>
-        <v>15.434181818181818</v>
+        <v>16.406545454545459</v>
       </c>
       <c r="G10" s="24">
         <f t="shared" si="2"/>
-        <v>16.034181818181818</v>
+        <v>17.00654545454546</v>
       </c>
       <c r="H10" s="24">
         <f t="shared" si="2"/>
-        <v>17.43418181818182</v>
+        <v>18.406545454545459</v>
       </c>
       <c r="I10" s="24">
         <f t="shared" si="2"/>
-        <v>4.4341818181818189</v>
+        <v>5.4065454545454568</v>
       </c>
       <c r="J10" s="24">
         <f t="shared" si="2"/>
-        <v>4.4341818181818189</v>
+        <v>5.4065454545454568</v>
       </c>
       <c r="K10" s="24">
         <f t="shared" si="2"/>
-        <v>4.4341818181818189</v>
+        <v>5.4065454545454568</v>
       </c>
       <c r="L10" s="24">
         <f t="shared" si="2"/>
-        <v>4.4341818181818189</v>
+        <v>5.4065454545454568</v>
       </c>
       <c r="M10" s="24">
         <f t="shared" si="2"/>
-        <v>4.4341818181818189</v>
+        <v>5.4065454545454568</v>
       </c>
       <c r="N10" s="24">
         <f t="shared" si="2"/>
-        <v>4.4341818181818189</v>
+        <v>5.4065454545454568</v>
       </c>
       <c r="O10" s="24">
         <f t="shared" si="2"/>
-        <v>4.4341818181818189</v>
+        <v>5.4065454545454568</v>
       </c>
       <c r="P10" s="24">
         <f t="shared" si="2"/>
-        <v>4.4341818181818189</v>
+        <v>5.4065454545454568</v>
       </c>
       <c r="Q10" s="24">
         <f t="shared" si="2"/>
-        <v>4.4341818181818189</v>
+        <v>5.4065454545454568</v>
       </c>
       <c r="R10" s="29"/>
       <c r="S10" s="24"/>
@@ -4361,7 +4324,7 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -4379,8 +4342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C190218-096C-D04F-B5E6-6BE0B32B2632}">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4400,7 +4363,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="14"/>
@@ -4419,10 +4382,10 @@
     </row>
     <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C3" s="21">
         <f>'Group and Self Assessment'!C10</f>
@@ -4440,13 +4403,13 @@
         <f>'Group and Self Assessment'!C13</f>
         <v>1201384</v>
       </c>
-      <c r="G3" s="21">
+      <c r="G3" s="21" t="str">
         <f>'Group and Self Assessment'!C14</f>
-        <v>1180727</v>
-      </c>
-      <c r="H3" s="21">
+        <v>Student 5</v>
+      </c>
+      <c r="H3" s="21" t="str">
         <f>'Group and Self Assessment'!C15</f>
-        <v>1200801</v>
+        <v>Student 6</v>
       </c>
       <c r="I3" s="21" t="str">
         <f>'Group and Self Assessment'!C16</f>
@@ -4512,7 +4475,7 @@
         <v>5</v>
       </c>
       <c r="Y3" s="22" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="Z3" s="12" t="s">
         <v>30</v>
@@ -4520,7 +4483,7 @@
     </row>
     <row r="4" spans="1:26" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B4" s="18">
         <v>0.1</v>
@@ -4557,29 +4520,29 @@
         <v>3</v>
       </c>
       <c r="S4" s="74" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="T4" s="74" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="U4" s="74" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="V4" s="74" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="W4" s="74" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="X4" s="74" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="Y4" s="71"/>
       <c r="Z4" s="16"/>
     </row>
     <row r="5" spans="1:26" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="B5" s="18">
         <v>0.1</v>
@@ -4616,29 +4579,29 @@
         <v>4</v>
       </c>
       <c r="S5" s="74" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="T5" s="74" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="U5" s="74" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="V5" s="74" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="W5" s="74" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="X5" s="74" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="Y5" s="71"/>
       <c r="Z5" s="16"/>
     </row>
     <row r="6" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B6" s="18">
         <v>0.05</v>
@@ -4675,29 +4638,29 @@
         <v>4</v>
       </c>
       <c r="S6" s="74" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="T6" s="74" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="U6" s="74" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="V6" s="74" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="W6" s="74" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="X6" s="74" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="Y6" s="71"/>
       <c r="Z6" s="16"/>
     </row>
     <row r="7" spans="1:26" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="B7" s="18">
         <v>0.05</v>
@@ -4734,29 +4697,29 @@
         <v>4</v>
       </c>
       <c r="S7" s="74" t="s">
+        <v>106</v>
+      </c>
+      <c r="T7" s="74" t="s">
+        <v>113</v>
+      </c>
+      <c r="U7" s="74" t="s">
+        <v>114</v>
+      </c>
+      <c r="V7" s="74" t="s">
+        <v>115</v>
+      </c>
+      <c r="W7" s="74" t="s">
+        <v>116</v>
+      </c>
+      <c r="X7" s="74" t="s">
         <v>117</v>
-      </c>
-      <c r="T7" s="74" t="s">
-        <v>124</v>
-      </c>
-      <c r="U7" s="74" t="s">
-        <v>125</v>
-      </c>
-      <c r="V7" s="74" t="s">
-        <v>126</v>
-      </c>
-      <c r="W7" s="74" t="s">
-        <v>127</v>
-      </c>
-      <c r="X7" s="74" t="s">
-        <v>128</v>
       </c>
       <c r="Y7" s="71"/>
       <c r="Z7" s="16"/>
     </row>
     <row r="8" spans="1:26" ht="63" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="B8" s="18">
         <v>0.1</v>
@@ -4793,50 +4756,50 @@
         <v>3.1666666666666665</v>
       </c>
       <c r="S8" s="74" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="T8" s="74" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="U8" s="74" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="V8" s="74" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="W8" s="74" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="X8" s="74" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="Y8" s="71"/>
       <c r="Z8" s="16"/>
     </row>
     <row r="9" spans="1:26" ht="63" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B9" s="18">
         <v>0.05</v>
       </c>
       <c r="C9" s="26">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D9" s="26">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E9" s="26">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F9" s="26">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G9" s="26">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H9" s="26">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I9" s="26"/>
       <c r="J9" s="26"/>
@@ -4849,28 +4812,28 @@
       <c r="Q9" s="26"/>
       <c r="R9" s="70">
         <f t="shared" ref="R9:R11" si="2">AVERAGE(C9:Q9)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="S9" s="74" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="T9" s="74" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="U9" s="74"/>
       <c r="V9" s="74" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="W9" s="74"/>
       <c r="X9" s="74" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="Y9" s="71"/>
       <c r="Z9" s="16"/>
     </row>
     <row r="10" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="B10" s="18">
         <v>0.1</v>
@@ -4907,29 +4870,29 @@
         <v>5</v>
       </c>
       <c r="S10" s="74" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="T10" s="74" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="U10" s="74" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="V10" s="74" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="W10" s="74" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="X10" s="74" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="Y10" s="71"/>
       <c r="Z10" s="16"/>
     </row>
     <row r="11" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="B11" s="18">
         <v>0.1</v>
@@ -4966,29 +4929,29 @@
         <v>3</v>
       </c>
       <c r="S11" s="74" t="s">
+        <v>125</v>
+      </c>
+      <c r="T11" s="74" t="s">
         <v>136</v>
       </c>
-      <c r="T11" s="74" t="s">
-        <v>147</v>
-      </c>
       <c r="U11" s="74" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="V11" s="74" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="W11" s="74" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="X11" s="74" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="Y11" s="71"/>
       <c r="Z11" s="16"/>
     </row>
     <row r="12" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="B12" s="18">
         <v>0.1</v>
@@ -5025,29 +4988,29 @@
         <v>5</v>
       </c>
       <c r="S12" s="74" t="s">
+        <v>125</v>
+      </c>
+      <c r="T12" s="74" t="s">
         <v>136</v>
       </c>
-      <c r="T12" s="74" t="s">
-        <v>147</v>
-      </c>
       <c r="U12" s="74" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="V12" s="74" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="W12" s="74" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="X12" s="74" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="Y12" s="71"/>
       <c r="Z12" s="16"/>
     </row>
     <row r="13" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="B13" s="18">
         <v>0.1</v>
@@ -5084,29 +5047,29 @@
         <v>4.166666666666667</v>
       </c>
       <c r="S13" s="74" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="T13" s="74" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="U13" s="74" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="V13" s="74" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="W13" s="74" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="X13" s="74" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="Y13" s="71"/>
       <c r="Z13" s="16"/>
     </row>
     <row r="14" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="B14" s="18">
         <v>0.15</v>
@@ -5143,29 +5106,29 @@
         <v>5</v>
       </c>
       <c r="S14" s="74" t="s">
+        <v>125</v>
+      </c>
+      <c r="T14" s="74" t="s">
         <v>136</v>
       </c>
-      <c r="T14" s="74" t="s">
-        <v>147</v>
-      </c>
       <c r="U14" s="74" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="V14" s="74" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="W14" s="74" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="X14" s="74" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="Y14" s="71"/>
       <c r="Z14" s="16"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B15" s="19">
         <f>SUM(B4:B14)</f>
@@ -5173,27 +5136,27 @@
       </c>
       <c r="C15" s="7">
         <f t="shared" ref="C15:Q15" si="4">SUMPRODUCT(C8:C14,$B$8:$B$14)</f>
-        <v>3</v>
+        <v>2.8000000000000003</v>
       </c>
       <c r="D15" s="7">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>2.8000000000000003</v>
       </c>
       <c r="E15" s="7">
         <f t="shared" si="4"/>
-        <v>3.1</v>
+        <v>2.9</v>
       </c>
       <c r="F15" s="7">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>2.8000000000000003</v>
       </c>
       <c r="G15" s="7">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>2.8000000000000003</v>
       </c>
       <c r="H15" s="7">
         <f t="shared" si="4"/>
-        <v>3.1</v>
+        <v>2.9000000000000004</v>
       </c>
       <c r="I15" s="7">
         <f t="shared" si="4"/>
@@ -5243,32 +5206,32 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B16" s="24"/>
       <c r="C16" s="24">
         <f>C15/5*20</f>
-        <v>12</v>
+        <v>11.200000000000001</v>
       </c>
       <c r="D16" s="24">
         <f t="shared" ref="D16:Q16" si="5">D15/5*20</f>
-        <v>12</v>
+        <v>11.200000000000001</v>
       </c>
       <c r="E16" s="24">
         <f t="shared" si="5"/>
-        <v>12.4</v>
+        <v>11.6</v>
       </c>
       <c r="F16" s="24">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>11.200000000000001</v>
       </c>
       <c r="G16" s="24">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>11.200000000000001</v>
       </c>
       <c r="H16" s="24">
         <f t="shared" si="5"/>
-        <v>12.4</v>
+        <v>11.600000000000001</v>
       </c>
       <c r="I16" s="24">
         <f t="shared" si="5"/>
@@ -5318,7 +5281,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -5354,6 +5317,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005836243B3C47804EAF5FFDD9F066FCC7" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9d21ddf3f0b128e39c9d770c8c903166">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0326308c339679ad994635f2c691325" ns2:_="">
     <xsd:import namespace="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
@@ -5537,12 +5506,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
   <ds:schemaRefs>
@@ -5552,6 +5515,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CA1CEFC-B112-44A5-8B0C-097F64092DA8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5567,20 +5546,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
G41-98 #comment Updating self assessment
</commit_message>
<xml_diff>
--- a/LAPR3-2021-Self-Assessment.xlsx
+++ b/LAPR3-2021-Self-Assessment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Desktop\Universidade-ISEP\2ANO\LAPR3\ProjetoIntegrador_G41\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92AC110B-1050-4CC1-A7A0-6AF9C88AD0F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525C4366-E54B-4017-8939-1D9F03AA3185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{5ECC33D7-267E-3941-AADB-18CFA00ADDCE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{5ECC33D7-267E-3941-AADB-18CFA00ADDCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="2" r:id="rId1"/>
@@ -2778,8 +2778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049E9D47-BAA1-5945-9716-C25FEE03B60C}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3124,7 +3124,7 @@
         <v>1201276</v>
       </c>
       <c r="C14" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D14" s="13"/>
       <c r="E14" s="15" t="s">
@@ -3699,8 +3699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20984BA6-2128-EB41-A750-F94245E6A6D5}">
   <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3952,12 +3952,8 @@
       <c r="F5" s="26">
         <v>3</v>
       </c>
-      <c r="G5" s="26">
-        <v>5</v>
-      </c>
-      <c r="H5" s="26">
-        <v>5</v>
-      </c>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
       <c r="I5" s="26"/>
       <c r="J5" s="26"/>
       <c r="K5" s="26"/>
@@ -3969,7 +3965,7 @@
       <c r="Q5" s="26"/>
       <c r="R5" s="28">
         <f t="shared" ref="R5:R8" si="0">AVERAGE(C5:Q5)</f>
-        <v>4.666666666666667</v>
+        <v>4.5</v>
       </c>
       <c r="S5" s="7" t="s">
         <v>64</v>
@@ -4011,12 +4007,8 @@
       <c r="F6" s="26">
         <v>5</v>
       </c>
-      <c r="G6" s="26">
-        <v>5</v>
-      </c>
-      <c r="H6" s="26">
-        <v>5</v>
-      </c>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
       <c r="I6" s="26"/>
       <c r="J6" s="26"/>
       <c r="K6" s="26"/>
@@ -4070,12 +4062,8 @@
       <c r="F7" s="26">
         <v>4</v>
       </c>
-      <c r="G7" s="26">
-        <v>4</v>
-      </c>
-      <c r="H7" s="26">
-        <v>5</v>
-      </c>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
       <c r="I7" s="26"/>
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
@@ -4087,7 +4075,7 @@
       <c r="Q7" s="26"/>
       <c r="R7" s="28">
         <f t="shared" si="0"/>
-        <v>4.166666666666667</v>
+        <v>4</v>
       </c>
       <c r="S7" s="7" t="s">
         <v>78</v>
@@ -4129,12 +4117,8 @@
       <c r="F8" s="26">
         <v>5</v>
       </c>
-      <c r="G8" s="26">
-        <v>5</v>
-      </c>
-      <c r="H8" s="26">
-        <v>5</v>
-      </c>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
       <c r="I8" s="26"/>
       <c r="J8" s="26"/>
       <c r="K8" s="26"/>
@@ -4195,11 +4179,11 @@
       </c>
       <c r="G9" s="7">
         <f t="shared" si="1"/>
-        <v>4.251636363636365</v>
+        <v>1.3516363636363644</v>
       </c>
       <c r="H9" s="7">
         <f t="shared" si="1"/>
-        <v>4.6016363636363646</v>
+        <v>1.3516363636363644</v>
       </c>
       <c r="I9" s="7">
         <f t="shared" si="1"/>
@@ -4270,11 +4254,11 @@
       </c>
       <c r="G10" s="24">
         <f t="shared" si="2"/>
-        <v>17.00654545454546</v>
+        <v>5.4065454545454568</v>
       </c>
       <c r="H10" s="24">
         <f t="shared" si="2"/>
-        <v>18.406545454545459</v>
+        <v>5.4065454545454568</v>
       </c>
       <c r="I10" s="24">
         <f t="shared" si="2"/>
@@ -4342,8 +4326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C190218-096C-D04F-B5E6-6BE0B32B2632}">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5317,12 +5301,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005836243B3C47804EAF5FFDD9F066FCC7" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9d21ddf3f0b128e39c9d770c8c903166">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0326308c339679ad994635f2c691325" ns2:_="">
     <xsd:import namespace="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
@@ -5506,6 +5484,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
   <ds:schemaRefs>
@@ -5515,22 +5499,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CA1CEFC-B112-44A5-8B0C-097F64092DA8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5546,4 +5514,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>